<commit_message>
update ml documentation ridge classifier
</commit_message>
<xml_diff>
--- a/ML Documentation/documentation.xlsx
+++ b/ML Documentation/documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaigu\Documents\repositories\DiabetesCapstone\ML Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1CC9AD-9157-460C-8177-00E0ED7370CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0D9A30-FD8E-47AD-A5A5-DA41E486A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="2100" windowWidth="11148" windowHeight="10260" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
+    <workbookView xWindow="-4224" yWindow="7020" windowWidth="9132" windowHeight="10260" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="10">
   <si>
     <t>Model</t>
   </si>
@@ -60,17 +60,17 @@
     <t>Score</t>
   </si>
   <si>
-    <t>Med Specialty Top 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drop </t>
+    <t>Drop Emergency</t>
+  </si>
+  <si>
+    <t>Drop Medical Specialty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,20 +79,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Var(--jp-code-font-family)"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
@@ -118,15 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CBF0B8-CF14-4846-958C-916F0354E86E}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -453,6 +436,7 @@
     <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -469,13 +453,13 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -491,7 +475,13 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2">
         <v>0.57886061190849503</v>
       </c>
     </row>
@@ -508,7 +498,13 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>0.58380573312427098</v>
       </c>
     </row>
@@ -525,7 +521,13 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
         <v>0.63963602301619105</v>
       </c>
     </row>
@@ -542,7 +544,13 @@
       <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.64993978321959001</v>
       </c>
     </row>
@@ -559,8 +567,14 @@
       <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="1">
-        <v>0.63997056068513303</v>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.64077345109059203</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -576,8 +590,62 @@
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
         <v>0.65067576609126099</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.64893617021276595</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.64732650739476605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add random forrest documentation
</commit_message>
<xml_diff>
--- a/ML Documentation/documentation.xlsx
+++ b/ML Documentation/documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaigu\Documents\repositories\DiabetesCapstone\ML Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0D9A30-FD8E-47AD-A5A5-DA41E486A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B640B07-546C-4972-9CFA-EB0C7B276CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4224" yWindow="7020" windowWidth="9132" windowHeight="10260" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="13">
   <si>
     <t>Model</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Encode MedList</t>
   </si>
   <si>
-    <t>Tune: Alpha = 88</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
@@ -64,13 +61,25 @@
   </si>
   <si>
     <t>Drop Medical Specialty</t>
+  </si>
+  <si>
+    <t>Tuned</t>
+  </si>
+  <si>
+    <t>Random Forest Classifier</t>
+  </si>
+  <si>
+    <t>Refactor MedList (Y/N)</t>
+  </si>
+  <si>
+    <t>Percent Improvement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +88,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
@@ -104,12 +127,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CBF0B8-CF14-4846-958C-916F0354E86E}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -435,11 +462,14 @@
     <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
@@ -461,8 +491,14 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -476,16 +512,23 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
         <v>0.57886061190849503</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <f>(H2-$H$2)/$H$2*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -496,19 +539,26 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
         <v>0.58380573312427098</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="0">(H3-$H$2)/$H$2*100</f>
+        <v>0.854285317405162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -522,16 +572,23 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.63963602301619105</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>10.499144328946544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -542,19 +599,26 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.64993978321959001</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>12.279151465626239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -568,40 +632,53 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.64077345109059203</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>10.695638623255306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
         <v>0.65067576609126099</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>12.406294832531866</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -611,7 +688,7 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -620,12 +697,19 @@
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.64893617021276595</v>
       </c>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>12.105774147118566</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -635,17 +719,204 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>3</v>
+      <c r="D9" t="s">
+        <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.64732650739476605</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>11.827699808515208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.64940452294928397</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>12.186683562422168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.58420777549953695</v>
+      </c>
+      <c r="I11">
+        <f>(H11-$H$11)/$H$11*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.64527872582480095</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I15" si="1">(H12-$H$11)/$H$11*100</f>
+        <v>10.45363531374505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.65000669075337802</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>11.262930418476298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.64873544761140101</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>11.045329216422797</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.65522547838886602</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="1"/>
+        <v>12.156240616380732</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated document to include KNN Classifier
</commit_message>
<xml_diff>
--- a/ML Documentation/documentation.xlsx
+++ b/ML Documentation/documentation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaigu\Documents\repositories\DiabetesCapstone\ML Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddy Doering\Documents\Random Junk\Summer Job\Job\GENESIS10\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B640B07-546C-4972-9CFA-EB0C7B276CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B01FE078-E193-44D3-899F-78DF72E06D8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
   <si>
     <t>Model</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>Percent Improvement</t>
+  </si>
+  <si>
+    <t>KNN Classifier</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Drop BUT "Internal Medicine" Medical Specalty</t>
+  </si>
+  <si>
+    <t>Drop "?" Medical Specalty</t>
+  </si>
+  <si>
+    <t>Drop "Emergency/Trama" Medical Specalty</t>
   </si>
 </sst>
 </file>
@@ -127,16 +145,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,22 +487,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CBF0B8-CF14-4846-958C-916F0354E86E}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B20" sqref="B20:K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -502,28 +539,28 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2">
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5">
         <v>0.57886061190849503</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <f>(H2-$H$2)/$H$2*100</f>
         <v>0</v>
       </c>
@@ -532,28 +569,28 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
         <v>0.58380573312427098</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <f t="shared" ref="I3:I10" si="0">(H3-$H$2)/$H$2*100</f>
         <v>0.854285317405162</v>
       </c>
@@ -562,28 +599,28 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6">
         <v>0.63963602301619105</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <f t="shared" si="0"/>
         <v>10.499144328946544</v>
       </c>
@@ -592,28 +629,28 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="1">
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6">
         <v>0.64993978321959001</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <f t="shared" si="0"/>
         <v>12.279151465626239</v>
       </c>
@@ -622,302 +659,638 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="1">
+      <c r="B6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6">
         <v>0.64077345109059203</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <f t="shared" si="0"/>
         <v>10.695638623255306</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8">
         <v>0.65067576609126099</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="7">
         <f t="shared" si="0"/>
         <v>12.406294832531866</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="B8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6">
         <v>0.64893617021276595</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <f t="shared" si="0"/>
         <v>12.105774147118566</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="1">
+      <c r="B9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="6">
         <v>0.64732650739476605</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <f t="shared" si="0"/>
         <v>11.827699808515208</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="1">
+      <c r="B10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="6">
         <v>0.64940452294928397</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <f t="shared" si="0"/>
         <v>12.186683562422168</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="1">
+      <c r="B11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="6">
         <v>0.58420777549953695</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <f>(H11-$H$11)/$H$11*100</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1">
+      <c r="B12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="6">
         <v>0.64527872582480095</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <f t="shared" ref="I12:I15" si="1">(H12-$H$11)/$H$11*100</f>
         <v>10.45363531374505</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="B13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="6">
         <v>0.65000669075337802</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <f t="shared" si="1"/>
         <v>11.262930418476298</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="1">
+      <c r="B14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="6">
         <v>0.64873544761140101</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <f t="shared" si="1"/>
         <v>11.045329216422797</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="B15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="8">
         <v>0.65522547838886602</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="7">
         <f t="shared" si="1"/>
         <v>12.156240616380732</v>
       </c>
+    </row>
+    <row r="19" spans="1:12" ht="47.25" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0.49330924662116898</v>
+      </c>
+      <c r="K20" s="3">
+        <f>(J20-$J$20)/$J$20*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.49484811989830002</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" ref="K21:K27" si="2">(J21-$J$20)/$J$20*100</f>
+        <v>0.3119490031194968</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.492573263749498</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="2"/>
+        <v>-0.14919300149185544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="3">
+        <v>0.568714037200588</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="2"/>
+        <v>15.285501152854982</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="2"/>
+        <v>19.600434016004471</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.58624381105312395</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="2"/>
+        <v>18.839007188390081</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.63648468708388795</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" si="2"/>
+        <v>29.023465796226773</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="3">
+        <v>0.61492537313432805</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" si="2"/>
+        <v>24.653121210710395</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added SGD Classifier to ML Documentation
</commit_message>
<xml_diff>
--- a/ML Documentation/documentation.xlsx
+++ b/ML Documentation/documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eddy Doering\Documents\Random Junk\Summer Job\Job\GENESIS10\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B01FE078-E193-44D3-899F-78DF72E06D8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED4D21D-175D-4096-9E06-731A1261D8A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
+    <workbookView xWindow="4950" yWindow="2010" windowWidth="21600" windowHeight="11385" xr2:uid="{550B15EF-57D2-4D11-B126-3EE559BB08A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="20">
   <si>
     <t>Model</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>Drop "Emergency/Trama" Medical Specalty</t>
+  </si>
+  <si>
+    <t>SGD Classifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +127,18 @@
       <color theme="1"/>
       <name val="Var(--jp-code-font-family)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Var(--jp-code-font-family)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -145,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -172,6 +187,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CBF0B8-CF14-4846-958C-916F0354E86E}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:K28"/>
+      <selection activeCell="H16" sqref="H16:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -956,292 +981,214 @@
         <v>12.156240616380732</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="47.25" customHeight="1">
-      <c r="A19" s="3" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.54352625799999998</v>
+      </c>
+      <c r="I16" s="12">
         <v>0</v>
       </c>
-      <c r="B19" s="4" t="s">
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0.54645599600000005</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.53902433100000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="12.75" customHeight="1">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0.55007437800000003</v>
+      </c>
+      <c r="I18" s="12">
+        <v>1.2047477120000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H19" s="14">
+        <v>0.60221927399999997</v>
+      </c>
+      <c r="I19" s="12">
+        <v>10.798561319999999</v>
+      </c>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="14">
+        <v>0.60792827599999999</v>
+      </c>
+      <c r="I20" s="12">
+        <v>11.84892488</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="12">
+        <v>0.63233224799999999</v>
+      </c>
+      <c r="I21" s="12">
+        <v>16.338859230000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="45">
+      <c r="A26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K26" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.49330924662116898</v>
-      </c>
-      <c r="K20" s="3">
-        <f>(J20-$J$20)/$J$20*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0.49484811989830002</v>
-      </c>
-      <c r="K21" s="3">
-        <f t="shared" ref="K21:K27" si="2">(J21-$J$20)/$J$20*100</f>
-        <v>0.3119490031194968</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.492573263749498</v>
-      </c>
-      <c r="K22" s="3">
-        <f t="shared" si="2"/>
-        <v>-0.14919300149185544</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0.568714037200588</v>
-      </c>
-      <c r="K23" s="3">
-        <f t="shared" si="2"/>
-        <v>15.285501152854982</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="3">
-        <v>0.59</v>
-      </c>
-      <c r="K24" s="3">
-        <f t="shared" si="2"/>
-        <v>19.600434016004471</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J25" s="3">
-        <v>0.58624381105312395</v>
-      </c>
-      <c r="K25" s="3">
-        <f t="shared" si="2"/>
-        <v>18.839007188390081</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="3">
-        <v>0.63648468708388795</v>
-      </c>
-      <c r="K26" s="3">
-        <f t="shared" si="2"/>
-        <v>29.023465796226773</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1249,48 +1196,288 @@
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="J27" s="3">
+        <v>0.49330924662116898</v>
+      </c>
+      <c r="K27" s="3">
+        <f>(J27-$J$27)/$J$27*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.49484811989830002</v>
+      </c>
+      <c r="K28" s="3">
+        <f>(J28-$J$27)/$J$27*100</f>
+        <v>0.3119490031194968</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0.492573263749498</v>
+      </c>
+      <c r="K29" s="3">
+        <f>(J29-$J$27)/$J$27*100</f>
+        <v>-0.14919300149185544</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.568714037200588</v>
+      </c>
+      <c r="K30" s="3">
+        <f>(J30-$J$27)/$J$27*100</f>
+        <v>15.285501152854982</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="K31" s="3">
+        <f>(J31-$J$27)/$J$27*100</f>
+        <v>19.600434016004471</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0.58624381105312395</v>
+      </c>
+      <c r="K32" s="3">
+        <f>(J32-$J$27)/$J$27*100</f>
+        <v>18.839007188390081</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0.63648468708388795</v>
+      </c>
+      <c r="K33" s="3">
+        <f>(J33-$J$27)/$J$27*100</f>
+        <v>29.023465796226773</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="3">
         <v>0.61492537313432805</v>
       </c>
-      <c r="K27" s="3">
-        <f t="shared" si="2"/>
+      <c r="K34" s="3">
+        <f>(J34-$J$27)/$J$27*100</f>
         <v>24.653121210710395</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>